<commit_message>
SUCCESS: Switched to Capture & Process, detection working on physical  Samsung
</commit_message>
<xml_diff>
--- a/PRELOAD DATA.xlsx
+++ b/PRELOAD DATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vighnesh\OneDrive\Desktop\Projects\Plate detection\Vibes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vighnesh\Desktop\Projects\Vibes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{55953421-66F6-4655-9F5E-113597A91B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A9638F-21EF-4864-8573-B82FB74D826B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{DB9EACCC-2B27-43B0-A55D-1F392C7B9637}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{DB9EACCC-2B27-43B0-A55D-1F392C7B9637}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>details</t>
   </si>
   <si>
-    <t>KA01MG1234</t>
-  </si>
-  <si>
     <t>Arjun Sharma</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Resident - Flat 402</t>
+  </si>
+  <si>
+    <t>MH20EJ0364</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,46 +485,46 @@
     </row>
     <row r="2" spans="1:3" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>